<commit_message>
get vitals, cards, set db
</commit_message>
<xml_diff>
--- a/guan_tbl.xlsx
+++ b/guan_tbl.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="13140" windowHeight="5820"/>
+    <workbookView windowWidth="19380" windowHeight="10365"/>
   </bookViews>
   <sheets>
     <sheet name="guan_tbl" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="38">
   <si>
     <t>amount</t>
   </si>
@@ -26,6 +26,12 @@
   </si>
   <si>
     <t>type</t>
+  </si>
+  <si>
+    <t>coupon</t>
+  </si>
+  <si>
+    <t>tenure</t>
   </si>
   <si>
     <t>云南城投</t>
@@ -130,9 +136,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -151,6 +157,29 @@
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="3"/>
       <name val="宋体"/>
@@ -159,10 +188,25 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -175,14 +219,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -190,15 +234,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -213,14 +249,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -229,6 +265,13 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -243,44 +286,7 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -302,19 +308,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -326,157 +476,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -508,6 +514,26 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -523,17 +549,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -545,15 +560,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -595,10 +601,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -607,133 +613,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1063,15 +1069,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D76"/>
+  <dimension ref="A1:F76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="5"/>
+  <cols>
+    <col min="2" max="2" width="11.5" customWidth="1"/>
+    <col min="5" max="5" width="13.75"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1084,8 +1094,14 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>260</v>
       </c>
@@ -1093,13 +1109,20 @@
         <v>43804</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>7</v>
+      </c>
+      <c r="E2">
+        <v>8</v>
+      </c>
+      <c r="F2">
+        <f>E2*2</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>56.29838142</v>
       </c>
@@ -1107,13 +1130,20 @@
         <v>43830</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>9</v>
+      </c>
+      <c r="E3">
+        <v>10</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F34" si="0">E3*2</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>48.2095</v>
       </c>
@@ -1121,13 +1151,20 @@
         <v>43823</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>11</v>
+      </c>
+      <c r="E4">
+        <v>9</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>42.9</v>
       </c>
@@ -1135,13 +1172,20 @@
         <v>43811</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>13</v>
+      </c>
+      <c r="E5">
+        <v>6</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>41</v>
       </c>
@@ -1149,13 +1193,20 @@
         <v>43813</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>7</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>38.8</v>
       </c>
@@ -1163,13 +1214,20 @@
         <v>43824</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+        <v>9</v>
+      </c>
+      <c r="E7">
+        <v>11</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>35.625</v>
       </c>
@@ -1177,13 +1235,20 @@
         <v>43809</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+        <v>11</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>32.46</v>
       </c>
@@ -1191,13 +1256,20 @@
         <v>43806</v>
       </c>
       <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" t="s">
         <v>13</v>
       </c>
-      <c r="D9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="E9">
+        <v>6</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>30.953379</v>
       </c>
@@ -1205,13 +1277,20 @@
         <v>43817</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+        <v>7</v>
+      </c>
+      <c r="E10">
+        <v>8</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>28</v>
       </c>
@@ -1219,13 +1298,20 @@
         <v>43827</v>
       </c>
       <c r="C11" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+        <v>9</v>
+      </c>
+      <c r="E11">
+        <v>10</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12">
         <v>27.7</v>
       </c>
@@ -1233,13 +1319,20 @@
         <v>43817</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
+        <v>11</v>
+      </c>
+      <c r="E12">
+        <v>9</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13">
         <v>26.3875</v>
       </c>
@@ -1247,13 +1340,20 @@
         <v>43827</v>
       </c>
       <c r="C13" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
+        <v>13</v>
+      </c>
+      <c r="E13">
+        <v>6</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14">
         <v>25</v>
       </c>
@@ -1261,13 +1361,20 @@
         <v>43816</v>
       </c>
       <c r="C14" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
+        <v>7</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15">
         <v>19.23225</v>
       </c>
@@ -1275,13 +1382,20 @@
         <v>43818</v>
       </c>
       <c r="C15" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
+        <v>9</v>
+      </c>
+      <c r="E15">
+        <v>11</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16">
         <v>16</v>
       </c>
@@ -1289,13 +1403,20 @@
         <v>43830</v>
       </c>
       <c r="C16" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+        <v>11</v>
+      </c>
+      <c r="E16">
+        <v>3</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17">
         <v>14.2</v>
       </c>
@@ -1303,13 +1424,20 @@
         <v>43806</v>
       </c>
       <c r="C17" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D17" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
+        <v>13</v>
+      </c>
+      <c r="E17">
+        <v>6</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18">
         <v>13.43</v>
       </c>
@@ -1317,13 +1445,20 @@
         <v>43813</v>
       </c>
       <c r="C18" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D18" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
+        <v>7</v>
+      </c>
+      <c r="E18">
+        <v>8</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19">
         <v>11</v>
       </c>
@@ -1331,13 +1466,20 @@
         <v>43830</v>
       </c>
       <c r="C19" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D19" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
+        <v>9</v>
+      </c>
+      <c r="E19">
+        <v>10</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20">
         <v>10.894</v>
       </c>
@@ -1345,13 +1487,20 @@
         <v>43806</v>
       </c>
       <c r="C20" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D20" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
+        <v>11</v>
+      </c>
+      <c r="E20">
+        <v>9</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21">
         <v>10.5</v>
       </c>
@@ -1359,13 +1508,20 @@
         <v>43804</v>
       </c>
       <c r="C21" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D21" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
+        <v>13</v>
+      </c>
+      <c r="E21">
+        <v>6</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22">
         <v>10.5</v>
       </c>
@@ -1373,13 +1529,20 @@
         <v>43804</v>
       </c>
       <c r="C22" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D22" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
+        <v>7</v>
+      </c>
+      <c r="E22">
+        <v>2</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23">
         <v>10</v>
       </c>
@@ -1387,13 +1550,20 @@
         <v>43803</v>
       </c>
       <c r="C23" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D23" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
+        <v>9</v>
+      </c>
+      <c r="E23">
+        <v>11</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24">
         <v>9.2</v>
       </c>
@@ -1401,13 +1571,20 @@
         <v>43830</v>
       </c>
       <c r="C24" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D24" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
+        <v>11</v>
+      </c>
+      <c r="E24">
+        <v>3</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25">
         <v>8.63</v>
       </c>
@@ -1415,13 +1592,20 @@
         <v>43802</v>
       </c>
       <c r="C25" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D25" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
+        <v>13</v>
+      </c>
+      <c r="E25">
+        <v>6</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26">
         <v>8</v>
       </c>
@@ -1429,13 +1613,20 @@
         <v>43812</v>
       </c>
       <c r="C26" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D26" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
+        <v>7</v>
+      </c>
+      <c r="E26">
+        <v>8</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27">
         <v>8</v>
       </c>
@@ -1443,13 +1634,20 @@
         <v>43820</v>
       </c>
       <c r="C27" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D27" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
+        <v>9</v>
+      </c>
+      <c r="E27">
+        <v>10</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28">
         <v>7.2</v>
       </c>
@@ -1457,13 +1655,20 @@
         <v>43827</v>
       </c>
       <c r="C28" t="s">
+        <v>20</v>
+      </c>
+      <c r="D28" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28">
+        <v>9</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="D28" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29">
         <v>7</v>
       </c>
@@ -1471,13 +1676,20 @@
         <v>43803</v>
       </c>
       <c r="C29" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D29" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
+        <v>13</v>
+      </c>
+      <c r="E29">
+        <v>6</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30">
         <v>7</v>
       </c>
@@ -1485,13 +1697,20 @@
         <v>43825</v>
       </c>
       <c r="C30" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D30" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
+        <v>7</v>
+      </c>
+      <c r="E30">
+        <v>2</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31">
         <v>7</v>
       </c>
@@ -1499,13 +1718,20 @@
         <v>43830</v>
       </c>
       <c r="C31" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D31" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
+        <v>9</v>
+      </c>
+      <c r="E31">
+        <v>11</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32">
         <v>6.12</v>
       </c>
@@ -1513,13 +1739,20 @@
         <v>43827</v>
       </c>
       <c r="C32" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D32" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
+        <v>11</v>
+      </c>
+      <c r="E32">
+        <v>3</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33">
         <v>6</v>
       </c>
@@ -1527,13 +1760,20 @@
         <v>43802</v>
       </c>
       <c r="C33" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D33" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
+        <v>13</v>
+      </c>
+      <c r="E33">
+        <v>6</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34">
         <v>5.6</v>
       </c>
@@ -1541,13 +1781,20 @@
         <v>43806</v>
       </c>
       <c r="C34" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D34" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
+        <v>7</v>
+      </c>
+      <c r="E34">
+        <v>8</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35">
         <v>5.4</v>
       </c>
@@ -1555,13 +1802,20 @@
         <v>43819</v>
       </c>
       <c r="C35" t="s">
+        <v>22</v>
+      </c>
+      <c r="D35" t="s">
+        <v>9</v>
+      </c>
+      <c r="E35">
+        <v>10</v>
+      </c>
+      <c r="F35">
+        <f t="shared" ref="F35:F66" si="1">E35*2</f>
         <v>20</v>
       </c>
-      <c r="D35" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
+    </row>
+    <row r="36" spans="1:6">
       <c r="A36">
         <v>5.25</v>
       </c>
@@ -1569,13 +1823,20 @@
         <v>43823</v>
       </c>
       <c r="C36" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D36" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
+        <v>11</v>
+      </c>
+      <c r="E36">
+        <v>9</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
       <c r="A37">
         <v>5</v>
       </c>
@@ -1583,13 +1844,20 @@
         <v>43820</v>
       </c>
       <c r="C37" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D37" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
+        <v>13</v>
+      </c>
+      <c r="E37">
+        <v>6</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
       <c r="A38">
         <v>5</v>
       </c>
@@ -1597,13 +1865,20 @@
         <v>43825</v>
       </c>
       <c r="C38" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D38" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
+        <v>7</v>
+      </c>
+      <c r="E38">
+        <v>2</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
       <c r="A39">
         <v>4.76</v>
       </c>
@@ -1611,13 +1886,20 @@
         <v>43823</v>
       </c>
       <c r="C39" t="s">
+        <v>24</v>
+      </c>
+      <c r="D39" t="s">
+        <v>9</v>
+      </c>
+      <c r="E39">
+        <v>11</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="D39" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
+    </row>
+    <row r="40" spans="1:6">
       <c r="A40">
         <v>4.63</v>
       </c>
@@ -1625,13 +1907,20 @@
         <v>43830</v>
       </c>
       <c r="C40" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D40" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
+        <v>11</v>
+      </c>
+      <c r="E40">
+        <v>3</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
       <c r="A41">
         <v>4.6</v>
       </c>
@@ -1639,13 +1928,20 @@
         <v>43806</v>
       </c>
       <c r="C41" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D41" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
+        <v>13</v>
+      </c>
+      <c r="E41">
+        <v>6</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
       <c r="A42">
         <v>4.5</v>
       </c>
@@ -1653,13 +1949,20 @@
         <v>43802</v>
       </c>
       <c r="C42" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D42" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
+        <v>7</v>
+      </c>
+      <c r="E42">
+        <v>8</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
       <c r="A43">
         <v>4.42</v>
       </c>
@@ -1667,13 +1970,20 @@
         <v>43820</v>
       </c>
       <c r="C43" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D43" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
+        <v>9</v>
+      </c>
+      <c r="E43">
+        <v>10</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
       <c r="A44">
         <v>4.42</v>
       </c>
@@ -1681,13 +1991,20 @@
         <v>43820</v>
       </c>
       <c r="C44" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D44" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
+        <v>7</v>
+      </c>
+      <c r="E44">
+        <v>9</v>
+      </c>
+      <c r="F44">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
       <c r="A45">
         <v>3.85</v>
       </c>
@@ -1695,13 +2012,20 @@
         <v>43823</v>
       </c>
       <c r="C45" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D45" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4">
+        <v>9</v>
+      </c>
+      <c r="E45">
+        <v>6</v>
+      </c>
+      <c r="F45">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
       <c r="A46">
         <v>3.234</v>
       </c>
@@ -1709,13 +2033,20 @@
         <v>43820</v>
       </c>
       <c r="C46" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D46" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
+        <v>11</v>
+      </c>
+      <c r="E46">
+        <v>2</v>
+      </c>
+      <c r="F46">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
       <c r="A47">
         <v>3</v>
       </c>
@@ -1723,13 +2054,20 @@
         <v>43823</v>
       </c>
       <c r="C47" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D47" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4">
+        <v>13</v>
+      </c>
+      <c r="E47">
+        <v>11</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
       <c r="A48">
         <v>3</v>
       </c>
@@ -1737,13 +2075,20 @@
         <v>43813</v>
       </c>
       <c r="C48" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D48" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4">
+        <v>7</v>
+      </c>
+      <c r="E48">
+        <v>3</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
       <c r="A49">
         <v>3</v>
       </c>
@@ -1751,13 +2096,20 @@
         <v>43827</v>
       </c>
       <c r="C49" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D49" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4">
+        <v>9</v>
+      </c>
+      <c r="E49">
+        <v>6</v>
+      </c>
+      <c r="F49">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
       <c r="A50">
         <v>3</v>
       </c>
@@ -1765,13 +2117,20 @@
         <v>43830</v>
       </c>
       <c r="C50" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D50" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4">
+        <v>11</v>
+      </c>
+      <c r="E50">
+        <v>8</v>
+      </c>
+      <c r="F50">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
       <c r="A51">
         <v>2.7</v>
       </c>
@@ -1779,13 +2138,20 @@
         <v>43820</v>
       </c>
       <c r="C51" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D51" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4">
+        <v>13</v>
+      </c>
+      <c r="E51">
+        <v>10</v>
+      </c>
+      <c r="F51">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
       <c r="A52">
         <v>2.5</v>
       </c>
@@ -1793,13 +2159,20 @@
         <v>43824</v>
       </c>
       <c r="C52" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D52" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4">
+        <v>7</v>
+      </c>
+      <c r="E52">
+        <v>9</v>
+      </c>
+      <c r="F52">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
       <c r="A53">
         <v>2.3</v>
       </c>
@@ -1807,13 +2180,20 @@
         <v>43820</v>
       </c>
       <c r="C53" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D53" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4">
+        <v>9</v>
+      </c>
+      <c r="E53">
+        <v>6</v>
+      </c>
+      <c r="F53">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
       <c r="A54">
         <v>2.1</v>
       </c>
@@ -1821,13 +2201,20 @@
         <v>43820</v>
       </c>
       <c r="C54" t="s">
+        <v>6</v>
+      </c>
+      <c r="D54" t="s">
+        <v>11</v>
+      </c>
+      <c r="E54">
+        <v>2</v>
+      </c>
+      <c r="F54">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="D54" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4">
+    </row>
+    <row r="55" spans="1:6">
       <c r="A55">
         <v>2.04</v>
       </c>
@@ -1835,13 +2222,20 @@
         <v>43809</v>
       </c>
       <c r="C55" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D55" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4">
+        <v>13</v>
+      </c>
+      <c r="E55">
+        <v>11</v>
+      </c>
+      <c r="F55">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
       <c r="A56">
         <v>2</v>
       </c>
@@ -1849,13 +2243,20 @@
         <v>43819</v>
       </c>
       <c r="C56" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D56" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4">
+        <v>7</v>
+      </c>
+      <c r="E56">
+        <v>3</v>
+      </c>
+      <c r="F56">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
       <c r="A57">
         <v>2</v>
       </c>
@@ -1863,13 +2264,20 @@
         <v>43819</v>
       </c>
       <c r="C57" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D57" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4">
+        <v>9</v>
+      </c>
+      <c r="E57">
+        <v>6</v>
+      </c>
+      <c r="F57">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
       <c r="A58">
         <v>2</v>
       </c>
@@ -1877,13 +2285,20 @@
         <v>43817</v>
       </c>
       <c r="C58" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D58" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4">
+        <v>11</v>
+      </c>
+      <c r="E58">
+        <v>8</v>
+      </c>
+      <c r="F58">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
       <c r="A59">
         <v>2</v>
       </c>
@@ -1891,13 +2306,20 @@
         <v>43830</v>
       </c>
       <c r="C59" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D59" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4">
+        <v>13</v>
+      </c>
+      <c r="E59">
+        <v>10</v>
+      </c>
+      <c r="F59">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
       <c r="A60">
         <v>1.56</v>
       </c>
@@ -1905,13 +2327,20 @@
         <v>43827</v>
       </c>
       <c r="C60" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D60" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4">
+        <v>7</v>
+      </c>
+      <c r="E60">
+        <v>9</v>
+      </c>
+      <c r="F60">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
       <c r="A61">
         <v>1.5</v>
       </c>
@@ -1919,13 +2348,20 @@
         <v>43830</v>
       </c>
       <c r="C61" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D61" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4">
+        <v>9</v>
+      </c>
+      <c r="E61">
+        <v>6</v>
+      </c>
+      <c r="F61">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
       <c r="A62">
         <v>1.42</v>
       </c>
@@ -1933,13 +2369,20 @@
         <v>43809</v>
       </c>
       <c r="C62" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D62" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4">
+        <v>11</v>
+      </c>
+      <c r="E62">
+        <v>2</v>
+      </c>
+      <c r="F62">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
       <c r="A63">
         <v>1.2</v>
       </c>
@@ -1947,13 +2390,20 @@
         <v>43827</v>
       </c>
       <c r="C63" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D63" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4">
+        <v>13</v>
+      </c>
+      <c r="E63">
+        <v>11</v>
+      </c>
+      <c r="F63">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
       <c r="A64">
         <v>1.0985</v>
       </c>
@@ -1961,13 +2411,20 @@
         <v>43802</v>
       </c>
       <c r="C64" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D64" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4">
+        <v>7</v>
+      </c>
+      <c r="E64">
+        <v>3</v>
+      </c>
+      <c r="F64">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
       <c r="A65">
         <v>1.05</v>
       </c>
@@ -1975,13 +2432,20 @@
         <v>43810</v>
       </c>
       <c r="C65" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D65" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4">
+        <v>9</v>
+      </c>
+      <c r="E65">
+        <v>6</v>
+      </c>
+      <c r="F65">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
       <c r="A66">
         <v>1</v>
       </c>
@@ -1989,13 +2453,20 @@
         <v>43813</v>
       </c>
       <c r="C66" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D66" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4">
+        <v>11</v>
+      </c>
+      <c r="E66">
+        <v>8</v>
+      </c>
+      <c r="F66">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
       <c r="A67">
         <v>0.9</v>
       </c>
@@ -2003,13 +2474,20 @@
         <v>43810</v>
       </c>
       <c r="C67" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D67" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4">
+        <v>13</v>
+      </c>
+      <c r="E67">
+        <v>10</v>
+      </c>
+      <c r="F67">
+        <f>E67*2</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
       <c r="A68">
         <v>0.88</v>
       </c>
@@ -2017,13 +2495,20 @@
         <v>43809</v>
       </c>
       <c r="C68" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D68" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4">
+        <v>7</v>
+      </c>
+      <c r="E68">
+        <v>9</v>
+      </c>
+      <c r="F68">
+        <f>E68*2</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
       <c r="A69">
         <v>0.8</v>
       </c>
@@ -2031,13 +2516,20 @@
         <v>43830</v>
       </c>
       <c r="C69" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D69" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4">
+        <v>9</v>
+      </c>
+      <c r="E69">
+        <v>6</v>
+      </c>
+      <c r="F69">
+        <f>E69*2</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
       <c r="A70">
         <v>0.75</v>
       </c>
@@ -2045,13 +2537,20 @@
         <v>43826</v>
       </c>
       <c r="C70" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D70" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4">
+        <v>11</v>
+      </c>
+      <c r="E70">
+        <v>2</v>
+      </c>
+      <c r="F70">
+        <f>E70*2</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6">
       <c r="A71">
         <v>0.54</v>
       </c>
@@ -2059,13 +2558,20 @@
         <v>43809</v>
       </c>
       <c r="C71" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D71" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4">
+        <v>13</v>
+      </c>
+      <c r="E71">
+        <v>11</v>
+      </c>
+      <c r="F71">
+        <f>E71*2</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
       <c r="A72">
         <v>0.5</v>
       </c>
@@ -2073,13 +2579,20 @@
         <v>43830</v>
       </c>
       <c r="C72" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D72" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4">
+        <v>7</v>
+      </c>
+      <c r="E72">
+        <v>3</v>
+      </c>
+      <c r="F72">
+        <f>E72*2</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6">
       <c r="A73">
         <v>0.33</v>
       </c>
@@ -2087,13 +2600,20 @@
         <v>43818</v>
       </c>
       <c r="C73" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D73" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4">
+        <v>9</v>
+      </c>
+      <c r="E73">
+        <v>6</v>
+      </c>
+      <c r="F73">
+        <f>E73*2</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6">
       <c r="A74">
         <v>0.3</v>
       </c>
@@ -2101,13 +2621,20 @@
         <v>43817</v>
       </c>
       <c r="C74" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D74" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4">
+        <v>11</v>
+      </c>
+      <c r="E74">
+        <v>8</v>
+      </c>
+      <c r="F74">
+        <f>E74*2</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6">
       <c r="A75">
         <v>0.23218</v>
       </c>
@@ -2115,13 +2642,20 @@
         <v>43810</v>
       </c>
       <c r="C75" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D75" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4">
+        <v>13</v>
+      </c>
+      <c r="E75">
+        <v>10</v>
+      </c>
+      <c r="F75">
+        <f>E75*2</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6">
       <c r="A76">
         <v>0.1</v>
       </c>
@@ -2129,10 +2663,17 @@
         <v>43826</v>
       </c>
       <c r="C76" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D76" t="s">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="E76">
+        <v>9</v>
+      </c>
+      <c r="F76">
+        <f>E76*2</f>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>